<commit_message>
iEMS test revision for using excel data provider, 2nd batch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218B427F-FFC3-4443-99F9-11022C98020B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B365136C-68C0-4389-8AEC-37F9E9CBF75A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
     <sheet name="getDeviceInfoByID" sheetId="6" r:id="rId2"/>
     <sheet name="getSensorByDeviceId" sheetId="7" r:id="rId3"/>
+    <sheet name="getSensorDataBySensorId" sheetId="9" r:id="rId4"/>
+    <sheet name="getSensorDataByDeviceId" sheetId="8" r:id="rId5"/>
+    <sheet name="getTopSensorDataByDeviceId" sheetId="10" r:id="rId6"/>
+    <sheet name="getKpiDataByDeviceId" sheetId="11" r:id="rId7"/>
+    <sheet name="getTopKPIDataByDeviceId" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -64,8 +69,102 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9C471DC1-975B-44FD-9FA4-A21727323D75}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{9C471DC1-975B-44FD-9FA4-A21727323D75}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The API expects a long integer which represents the count of milliseconds after 1970/01/01 (00:00:00 GMT). In order to improve readability, test case will use the normal time format and do the conversion automatically.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5DFE7C71-FED4-4AE6-B130-1FDA3DE5739C}</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5DFE7C71-FED4-4AE6-B130-1FDA3DE5739C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={E6B5C690-30C6-48D2-B76C-6B3A7EEEE79B}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{E6B5C690-30C6-48D2-B76C-6B3A7EEEE79B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={17967204-F501-4146-9A7D-D9F45ADBA235}</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{17967204-F501-4146-9A7D-D9F45ADBA235}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0330809A-1946-4DA7-9084-B833D2CC45D6}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{0330809A-1946-4DA7-9084-B833D2CC45D6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="55">
   <si>
     <t>description</t>
   </si>
@@ -158,6 +257,78 @@
   </si>
   <si>
     <t>busLine</t>
+  </si>
+  <si>
+    <t>endTime</t>
+  </si>
+  <si>
+    <t>startTime</t>
+  </si>
+  <si>
+    <t>2020-12-01 03:00:00</t>
+  </si>
+  <si>
+    <t>2020-11-27 04:00:00</t>
+  </si>
+  <si>
+    <t>sensor_id_list</t>
+  </si>
+  <si>
+    <t>bad request, startTime is missing</t>
+  </si>
+  <si>
+    <t>bad request, endTime is missing</t>
+  </si>
+  <si>
+    <t>bad request, sensor list is missing</t>
+  </si>
+  <si>
+    <t>35698,34159,34155</t>
+  </si>
+  <si>
+    <t>34159,34155</t>
+  </si>
+  <si>
+    <t>[endTime:endTime is null]</t>
+  </si>
+  <si>
+    <t>[startTime:startTime is null]</t>
+  </si>
+  <si>
+    <t>[sensor_list:sensor_list is null]</t>
+  </si>
+  <si>
+    <t>bad request, device id is missing</t>
+  </si>
+  <si>
+    <t>2020-11-27 04:00:01</t>
+  </si>
+  <si>
+    <t>[deviceId:deviceId is null]</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>[limit:limit not correct, should be number &lt; 1000]</t>
+  </si>
+  <si>
+    <t>[limit:limit is null]</t>
+  </si>
+  <si>
+    <t>bad request, limit is missing</t>
+  </si>
+  <si>
+    <t>bad request, limit value out of range</t>
+  </si>
+  <si>
+    <t>2020-09-27 04:00:00</t>
   </si>
 </sst>
 </file>
@@ -227,11 +398,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,11 +708,55 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2020-12-10T01:56:31.12" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{9C471DC1-975B-44FD-9FA4-A21727323D75}">
+    <text>The API expects a long integer which represents the count of milliseconds after 1970/01/01 (00:00:00 GMT). In order to improve readability, test case will use the normal time format and do the conversion automatically.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{5DFE7C71-FED4-4AE6-B130-1FDA3DE5739C}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{E6B5C690-30C6-48D2-B76C-6B3A7EEEE79B}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment6.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{17967204-F501-4146-9A7D-D9F45ADBA235}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment7.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{0330809A-1946-4DA7-9084-B833D2CC45D6}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0514F60E-1E6C-4713-A724-DC49130D4C9A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
@@ -802,7 +1020,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -933,4 +1151,836 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A9E2A3-C1DE-45EB-8CEF-E6F21F1688B8}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D2:D4" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E97B0C-4E25-4A95-A0C9-E33797A04BAD}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="20.6328125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.6328125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3">
+        <v>200</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3">
+        <v>200</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3">
+        <v>200</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>123456798</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3">
+        <v>200</v>
+      </c>
+      <c r="H6" s="3">
+        <v>102101</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC7F451-EA0B-481B-AAEE-BD37870611EA}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>123456798</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>200</v>
+      </c>
+      <c r="G6" s="3">
+        <v>102101</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3 E5" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6C785A-4057-490D-8636-A5D2A6B49506}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="20.6328125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.6328125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3">
+        <v>200</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="3">
+        <v>200</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3">
+        <v>200</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3">
+        <v>200</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>123456798</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="3">
+        <v>200</v>
+      </c>
+      <c r="H6" s="3">
+        <v>102101</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B9F9B-CFC3-492B-8FCA-7B8DEF2493D8}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.6328125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3">
+        <v>200</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="3">
+        <v>200</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="3">
+        <v>200</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>123456798</v>
+      </c>
+      <c r="E6" s="4">
+        <v>20</v>
+      </c>
+      <c r="F6" s="3">
+        <v>200</v>
+      </c>
+      <c r="G6" s="3">
+        <v>102101</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2:E3 E5" numberStoredAsText="1"/>
+  </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
iEMS test revision for using excel data provider, done
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B365136C-68C0-4389-8AEC-37F9E9CBF75A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D9C68D-7F62-40B3-AEF8-3CDEF3E21449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,10 @@
     <sheet name="getTopSensorDataByDeviceId" sheetId="10" r:id="rId6"/>
     <sheet name="getKpiDataByDeviceId" sheetId="11" r:id="rId7"/>
     <sheet name="getTopKPIDataByDeviceId" sheetId="12" r:id="rId8"/>
+    <sheet name="subscriptionsBySensorId" sheetId="13" r:id="rId9"/>
+    <sheet name="subscriptionsByDeviceId" sheetId="14" r:id="rId10"/>
+    <sheet name="subscriptionsWithKPIByDeviceId" sheetId="15" r:id="rId11"/>
+    <sheet name="deleteSubscriptions" sheetId="16" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -163,8 +167,46 @@
 </comments>
 </file>
 
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B1EE229D-3AC0-4A63-952D-2132D3852FF3}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{B1EE229D-3AC0-4A63-952D-2132D3852FF3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={84370DBC-6F5B-4400-8F93-55B8D945A994}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{84370DBC-6F5B-4400-8F93-55B8D945A994}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="78">
   <si>
     <t>description</t>
   </si>
@@ -329,6 +371,75 @@
   </si>
   <si>
     <t>2020-09-27 04:00:00</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>good request, operation success</t>
+  </si>
+  <si>
+    <t>bad request, sensor id is missing</t>
+  </si>
+  <si>
+    <t>bad request, incorrect data type</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bad request, separator is not comma</t>
+  </si>
+  <si>
+    <t>34155,34159,34155</t>
+  </si>
+  <si>
+    <t>34155;34159;34155</t>
+  </si>
+  <si>
+    <t>Required String parameter 'request' is not present</t>
+  </si>
+  <si>
+    <t>subscriptionsBySensorId.request: parameters are Integer need to be separated by commas</t>
+  </si>
+  <si>
+    <t>Required Integer parameter 'deviceId' is not present</t>
+  </si>
+  <si>
+    <t>bad request, device id value is invalid</t>
+  </si>
+  <si>
+    <t>deviceList</t>
+  </si>
+  <si>
+    <t>separator</t>
+  </si>
+  <si>
+    <t>[heatPumpDetail,1#制冷机] [heatPumpDetail,3#制冷机]</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>[invalid,aaa] [invalid,bbb]</t>
+  </si>
+  <si>
+    <t>subscriptionsWithKPIByDeviceId.request: parameters are Integer need to be separated by commas</t>
+  </si>
+  <si>
+    <t>bad request, subscription id is missing</t>
+  </si>
+  <si>
+    <t>bad request, subscription id not exist</t>
+  </si>
+  <si>
+    <t>Subscriptions not exist</t>
+  </si>
+  <si>
+    <t>115adce67b8f41888700812fee58d6cf8e</t>
+  </si>
+  <si>
+    <t>subscriptionId</t>
   </si>
 </sst>
 </file>
@@ -752,6 +863,24 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment8.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{B1EE229D-3AC0-4A63-952D-2132D3852FF3}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment9.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-12-09T07:21:38.66" personId="{7B02F430-DF90-446B-8CE2-F8BCDAE3B75C}" id="{84370DBC-6F5B-4400-8F93-55B8D945A994}">
+    <text>deviceType and deviceName will be used by the test case to extract the corresponding device id as input parameter;
+if no deviceType is specified, the value of deviceName will be directly used as the input parameter</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0514F60E-1E6C-4713-A724-DC49130D4C9A}">
   <dimension ref="A1:F5"/>
@@ -868,6 +997,334 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76532F20-62D7-47A4-8752-2E5ADEA862B4}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08798671-DED1-4851-A8DF-0C914FB8CC5D}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3">
+        <v>200</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772E3497-461A-4C37-8F81-E0F5BC2DAC30}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>200</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>200</v>
+      </c>
+      <c r="F3" s="3">
+        <v>102105</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="3">
+        <v>200</v>
+      </c>
+      <c r="F4" s="3">
+        <v>102105</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1824,7 +2281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B9F9B-CFC3-492B-8FCA-7B8DEF2493D8}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1983,4 +2440,120 @@
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBA4E32-F388-4A75-9239-EE7DF306288E}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6328125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3">
+        <v>200</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3">
+        <v>200</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1001</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3">
+        <v>200</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1001</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="3">
+        <v>200</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1001</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add snc test case, 1st batch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D9C68D-7F62-40B3-AEF8-3CDEF3E21449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BC9C99-280F-4CA2-8196-FF85BDCDDE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="110">
   <si>
     <t>description</t>
   </si>
@@ -440,6 +440,102 @@
   </si>
   <si>
     <t>subscriptionId</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-6</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-7</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-8</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-9</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-12</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-13</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-17</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-20</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-21</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-24</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-26</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-27</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-28</t>
+  </si>
+  <si>
+    <t>iems-api-service-sp5-29</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-6</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-7</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-8</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-11</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-12</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-13</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-14</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-17</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-18</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-21</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-22</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-24</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-26</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-27</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-29-var1</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-29-var2</t>
+  </si>
+  <si>
+    <t>iems-api-service-kpi-35</t>
   </si>
 </sst>
 </file>
@@ -887,7 +983,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1103,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1043,7 +1139,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
@@ -1111,7 +1209,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1147,7 +1245,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
@@ -1233,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772E3497-461A-4C37-8F81-E0F5BC2DAC30}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1270,7 +1370,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>88</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
@@ -1289,7 +1391,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>73</v>
       </c>
@@ -1335,7 +1439,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1371,7 +1475,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1498,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1519,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1538,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1476,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D99B74-3EF5-45AB-A31A-FC3FB4398B1A}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1513,7 +1625,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1570,7 +1684,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1587,7 +1703,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1604,6 +1722,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1615,7 +1734,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1655,7 +1774,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1679,7 +1800,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
@@ -1701,7 +1824,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1760,7 +1885,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1802,7 +1927,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +1956,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
@@ -1854,7 +1983,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
@@ -1939,7 +2070,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1978,7 +2109,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2002,7 +2135,9 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>44</v>
       </c>
@@ -2022,7 +2157,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
@@ -2044,7 +2181,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
       </c>
@@ -2068,7 +2207,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2104,7 +2245,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2146,7 +2287,9 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2173,7 +2316,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
@@ -2198,7 +2343,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
@@ -2246,7 +2393,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2282,7 +2431,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2321,7 +2470,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2365,7 +2516,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
@@ -2387,7 +2540,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
       </c>
@@ -2411,7 +2566,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
@@ -2447,7 +2604,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2480,7 +2637,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
       </c>
@@ -2514,7 +2673,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>91</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
adjust error code and message for connector test with not exist order input
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F40D3B1-FE35-4829-BC4E-0A89519A4E90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F507F6-258E-4F5F-A1FD-D92502D9F738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="113">
   <si>
     <t>description</t>
   </si>
@@ -433,9 +433,6 @@
     <t>bad request, subscription id not exist</t>
   </si>
   <si>
-    <t>Subscriptions not exist</t>
-  </si>
-  <si>
     <t>115adce67b8f41888700812fee58d6cf8e</t>
   </si>
   <si>
@@ -542,6 +539,12 @@
   </si>
   <si>
     <t>2020-12-17 15:00:00</t>
+  </si>
+  <si>
+    <t>Subscription 115adce67b8f41888700812fee58d6cf8e not exists!</t>
+  </si>
+  <si>
+    <t>Subscription null not exists!</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1149,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
@@ -1252,7 +1255,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
@@ -1339,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772E3497-461A-4C37-8F81-E0F5BC2DAC30}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1363,7 +1366,7 @@
         <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1377,7 +1380,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
@@ -1398,7 +1401,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>73</v>
@@ -1409,10 +1412,10 @@
         <v>200</v>
       </c>
       <c r="F3" s="3">
-        <v>102105</v>
+        <v>500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1422,16 +1425,16 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="3">
         <v>200</v>
       </c>
       <c r="F4" s="3">
-        <v>102105</v>
+        <v>500</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1505,7 +1508,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1526,7 +1529,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
@@ -1545,7 +1548,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
@@ -1632,7 +1635,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1691,7 +1694,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>23</v>
@@ -1710,7 +1713,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -1781,7 +1784,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1807,7 +1810,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -1831,7 +1834,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -1934,7 +1937,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1963,7 +1966,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -1990,7 +1993,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -2116,7 +2119,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -2142,7 +2145,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2164,7 +2167,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -2188,7 +2191,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
@@ -2214,7 +2217,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2250,7 +2253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6C785A-4057-490D-8636-A5D2A6B49506}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2294,13 +2297,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -2309,7 +2312,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -2323,7 +2326,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>37</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -2400,7 +2403,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2477,7 +2480,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -2523,7 +2526,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
@@ -2547,7 +2550,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>53</v>
@@ -2573,7 +2576,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2644,7 +2647,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>56</v>
@@ -2680,7 +2683,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
change start/end time input for api serivce tests, e.g. getSensorDataByDeviceId
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F507F6-258E-4F5F-A1FD-D92502D9F738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03C046D-40FC-4AB9-9FF6-DB9C4ABDC52D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
   <si>
     <t>description</t>
   </si>
@@ -535,16 +535,25 @@
     <t>iems-api-service-kpi-35</t>
   </si>
   <si>
-    <t>2020-10-27 04:00:00</t>
-  </si>
-  <si>
-    <t>2020-12-17 15:00:00</t>
-  </si>
-  <si>
     <t>Subscription 115adce67b8f41888700812fee58d6cf8e not exists!</t>
   </si>
   <si>
     <t>Subscription null not exists!</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:00:00</t>
+  </si>
+  <si>
+    <t>2021-1-27 04:00:00</t>
+  </si>
+  <si>
+    <t>2020-12-27 04:00:00</t>
+  </si>
+  <si>
+    <t>2021-06-17 03:00:00</t>
+  </si>
+  <si>
+    <t>2021-6-17 03:00:00</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772E3497-461A-4C37-8F81-E0F5BC2DAC30}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1415,7 +1424,7 @@
         <v>500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1434,7 +1443,7 @@
         <v>500</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1742,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A9E2A3-C1DE-45EB-8CEF-E6F21F1688B8}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1790,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3">
         <v>200</v>
@@ -1894,7 +1903,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1943,7 +1952,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -1952,7 +1961,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -2254,7 +2263,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2303,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -2312,7 +2321,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>

</xml_diff>

<commit_message>
update test case base on SDL-4506,4507
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C03C046D-40FC-4AB9-9FF6-DB9C4ABDC52D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B626AE3-229C-48EC-8CC5-43DBB74AB1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2676" yWindow="3288" windowWidth="17280" windowHeight="10044" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="115">
   <si>
     <t>description</t>
   </si>
@@ -544,41 +544,47 @@
     <t>2021-06-17 15:00:00</t>
   </si>
   <si>
-    <t>2021-1-27 04:00:00</t>
-  </si>
-  <si>
     <t>2020-12-27 04:00:00</t>
   </si>
   <si>
-    <t>2021-06-17 03:00:00</t>
-  </si>
-  <si>
-    <t>2021-6-17 03:00:00</t>
+    <t>2017-11-06 08:13:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024-03-09 03:46:40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1004,14 +1010,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="12.6328125" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1124,16 +1130,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -1179,7 +1185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1196,7 +1202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1216,6 +1222,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1230,16 +1237,16 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -1283,7 +1290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1300,7 +1307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1319,7 +1326,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>66</v>
@@ -1341,6 +1348,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1355,16 +1363,16 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -1408,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
@@ -1427,7 +1435,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>74</v>
@@ -1447,6 +1455,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1460,16 +1469,16 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1492,7 +1501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>104</v>
       </c>
@@ -1515,7 +1524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>106</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>107</v>
       </c>
@@ -1555,7 +1564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -1596,6 +1605,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1610,16 +1620,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6328125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1642,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1684,7 +1694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -1701,7 +1711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>78</v>
       </c>
@@ -1720,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
@@ -1752,20 +1762,20 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.6328125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="20.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1799,13 +1809,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F2" s="3">
         <v>200</v>
@@ -1817,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>82</v>
       </c>
@@ -1841,7 +1851,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1865,7 +1875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>38</v>
@@ -1903,19 +1913,19 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="20.6328125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="12.6328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.6328125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1944,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>83</v>
       </c>
@@ -1961,7 +1971,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -1973,7 +1983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>85</v>
       </c>
@@ -2000,7 +2010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -2027,7 +2037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2050,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2091,16 +2101,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="20.6328125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2126,7 +2136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
@@ -2152,7 +2162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -2174,7 +2184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2198,7 +2208,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -2224,7 +2234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -2249,6 +2259,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
@@ -2266,16 +2277,16 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="6" width="20.6328125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="12.6328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.6328125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2304,7 +2315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -2321,7 +2332,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -2333,7 +2344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -2360,7 +2371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -2387,7 +2398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2410,7 +2421,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
@@ -2438,6 +2449,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -2452,16 +2464,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="5" width="20.6328125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2487,7 +2499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
@@ -2513,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2533,7 +2545,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>99</v>
       </c>
@@ -2557,7 +2569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>98</v>
       </c>
@@ -2583,7 +2595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -2608,6 +2620,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>
@@ -2625,16 +2638,16 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="12.6328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.6328125" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2654,7 +2667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>89</v>
       </c>
@@ -2674,7 +2687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>57</v>
@@ -2690,7 +2703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
@@ -2710,7 +2723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>60</v>
@@ -2729,6 +2742,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
update iems test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B626AE3-229C-48EC-8CC5-43DBB74AB1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65036F4-6CCE-43CD-8332-59826469321F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2676" yWindow="3288" windowWidth="17280" windowHeight="10044" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -559,30 +559,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1010,14 +1010,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1130,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1139,7 +1139,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1202,7 +1202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1237,7 +1237,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1246,7 +1246,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1307,7 +1307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1326,7 +1326,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>66</v>
@@ -1363,7 +1363,7 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1372,7 +1372,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>74</v>
@@ -1469,7 +1469,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1478,7 +1478,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>104</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>106</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>107</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -1620,7 +1620,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1629,7 +1629,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1694,7 +1694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -1711,7 +1711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>78</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
@@ -1761,11 +1761,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A9E2A3-C1DE-45EB-8CEF-E6F21F1688B8}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="6" customWidth="1"/>
@@ -1775,7 +1775,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>82</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>38</v>
@@ -1916,7 +1916,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
@@ -1925,7 +1925,7 @@
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>83</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>85</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2060,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2097,11 +2097,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC7F451-EA0B-481B-AAEE-BD37870611EA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
@@ -2110,7 +2110,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>200</v>
       </c>
       <c r="G6" s="3">
-        <v>102101</v>
+        <v>102102</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>12</v>
@@ -2277,7 +2277,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
@@ -2286,7 +2286,7 @@
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2421,7 +2421,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
@@ -2464,7 +2464,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
@@ -2473,7 +2473,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2545,7 +2545,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>99</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>98</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -2638,7 +2638,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
@@ -2647,7 +2647,7 @@
     <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>89</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>57</v>
@@ -2703,7 +2703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
update xlsx files which passed on feature-with-comment branch
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B626AE3-229C-48EC-8CC5-43DBB74AB1D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEEACA0-94BD-4B72-A72F-9B7D2FCE580D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2676" yWindow="3288" windowWidth="17280" windowHeight="10044" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -559,30 +559,30 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1010,14 +1010,14 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>28</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1130,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1139,7 +1139,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1202,7 +1202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1237,7 +1237,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1246,7 +1246,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>91</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -1307,7 +1307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>66</v>
@@ -1326,7 +1326,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>66</v>
@@ -1363,7 +1363,7 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1372,7 +1372,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>87</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>88</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>74</v>
@@ -1469,7 +1469,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1478,7 +1478,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>104</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>106</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>107</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>18</v>
@@ -1620,7 +1620,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
@@ -1629,7 +1629,7 @@
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>26</v>
@@ -1694,7 +1694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>17</v>
@@ -1711,7 +1711,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>78</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
         <v>79</v>
       </c>
@@ -1761,11 +1761,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A9E2A3-C1DE-45EB-8CEF-E6F21F1688B8}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="20.6640625" style="6" customWidth="1"/>
@@ -1775,7 +1775,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>82</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>38</v>
@@ -1916,7 +1916,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
@@ -1925,7 +1925,7 @@
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>83</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>85</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>84</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2060,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2097,11 +2097,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC7F451-EA0B-481B-AAEE-BD37870611EA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
@@ -2110,7 +2110,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>92</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>95</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>94</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -2252,10 +2252,10 @@
         <v>200</v>
       </c>
       <c r="G6" s="3">
-        <v>102101</v>
+        <v>102102</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2277,7 +2277,7 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
@@ -2286,7 +2286,7 @@
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>100</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>102</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>101</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>44</v>
@@ -2421,7 +2421,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
         <v>103</v>
       </c>
@@ -2464,7 +2464,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
@@ -2473,7 +2473,7 @@
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
@@ -2525,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>44</v>
@@ -2545,7 +2545,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
         <v>99</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
         <v>98</v>
       </c>
@@ -2595,7 +2595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>97</v>
       </c>
@@ -2638,7 +2638,7 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
@@ -2647,7 +2647,7 @@
     <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>89</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>57</v>
@@ -2703,7 +2703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>90</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
modify the port of Subscription,cases of Subscription
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEEACA0-94BD-4B72-A72F-9B7D2FCE580D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F594F69-6D11-48BD-B008-7F4829E6D561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="131">
   <si>
     <t>description</t>
   </si>
@@ -235,9 +235,6 @@
     <t>OK</t>
   </si>
   <si>
-    <t>iems-api-service-sp5-2</t>
-  </si>
-  <si>
     <t>bad request, incorrect device type</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
     <t>Device not exist</t>
   </si>
   <si>
-    <t>iems-api-service-sp5-3</t>
-  </si>
-  <si>
     <t>bad request, device type is missing in the request</t>
   </si>
   <si>
@@ -292,12 +286,6 @@
     <t>bad request, device id field not present in the request</t>
   </si>
   <si>
-    <t>iems-api-service-sp5-1-var1</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-1-var2</t>
-  </si>
-  <si>
     <t>busLine</t>
   </si>
   <si>
@@ -437,102 +425,6 @@
   </si>
   <si>
     <t>subscriptionId</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-6</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-7</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-8</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-9</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-12</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-13</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-17</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-20</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-21</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-24</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-26</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-27</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-28</t>
-  </si>
-  <si>
-    <t>iems-api-service-sp5-29</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-2</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-6</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-7</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-8</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-11</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-12</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-13</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-14</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-17</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-18</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-21</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-22</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-24</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-26</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-27</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-29-var1</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-29-var2</t>
-  </si>
-  <si>
-    <t>iems-api-service-kpi-35</t>
   </si>
   <si>
     <t>Subscription 115adce67b8f41888700812fee58d6cf8e not exists!</t>
@@ -553,6 +445,162 @@
   <si>
     <t>2024-03-09 03:46:40</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iems-api-service-getDevicesByType-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getDevicesByType-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getDevicesByType-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getDevicesByType-4</t>
+  </si>
+  <si>
+    <t>iems-api-servicegetDeviceInfoByID-1</t>
+  </si>
+  <si>
+    <t>iems-api-servicegetDeviceInfoByID-2</t>
+  </si>
+  <si>
+    <t>iems-api-servicegetDeviceInfoByID-3</t>
+  </si>
+  <si>
+    <t>iems-api-servicegetDeviceInfoByID-4</t>
+  </si>
+  <si>
+    <t>iems-api-servicegetDeviceInfoByID-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorByDeviceId-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataBySensorId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataBySensorId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataBySensorId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataBySensorId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getSensorDataByDeviceId-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopSensorDataByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopSensorDataByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopSensorDataByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopSensorDataByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopSensorDataByDeviceId-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-getKpiDataByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getKpiDataByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getKpiDataByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getKpiDataByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getKpiDataByDeviceId-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopKPIDataByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopKPIDataByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopKPIDataByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopKPIDataByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-getTopKPIDataByDeviceId-5</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsBySensorId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsBySensorId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsBySensorId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsBySensorId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsWithKPIByDeviceId-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsWithKPIByDeviceId-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsWithKPIByDeviceId-3</t>
+  </si>
+  <si>
+    <t>iems-api-service-subscriptionsWithKPIByDeviceId-4</t>
+  </si>
+  <si>
+    <t>iems-api-service-deleteSubscriptions-1</t>
+  </si>
+  <si>
+    <t>iems-api-service-deleteSubscriptions-2</t>
+  </si>
+  <si>
+    <t>iems-api-service-deleteSubscriptions-3</t>
   </si>
 </sst>
 </file>
@@ -1007,14 +1055,18 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="12.6640625" style="2"/>
+    <col min="1" max="1" width="30.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1039,7 +1091,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1059,13 +1111,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3">
         <v>200</v>
@@ -1079,13 +1131,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -1094,15 +1146,15 @@
         <v>102101</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
@@ -1112,7 +1164,7 @@
         <v>102101</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1127,15 +1179,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="34.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1150,7 +1205,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1164,16 +1219,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1186,9 +1241,11 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1199,17 +1256,19 @@
         <v>1001</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3">
         <v>200</v>
@@ -1218,7 +1277,7 @@
         <v>1001</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1233,16 +1292,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08798671-DED1-4851-A8DF-0C914FB8CC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="41.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="78.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1254,10 +1316,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1271,13 +1333,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>124</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
@@ -1291,9 +1353,11 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1304,16 +1368,18 @@
         <v>1001</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3">
@@ -1323,19 +1389,21 @@
         <v>1001</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E5" s="3">
         <v>200</v>
@@ -1344,7 +1412,7 @@
         <v>1001</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1360,15 +1428,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1380,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1397,13 +1468,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
@@ -1418,10 +1489,10 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1432,17 +1503,19 @@
         <v>500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E4" s="3">
         <v>200</v>
@@ -1451,7 +1524,7 @@
         <v>500</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1466,15 +1539,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1489,7 +1565,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1503,7 +1579,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1512,7 +1588,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1526,14 +1602,14 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
@@ -1542,15 +1618,15 @@
         <v>500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1561,15 +1637,15 @@
         <v>1001</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
@@ -1582,17 +1658,19 @@
         <v>102101</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3">
         <v>200</v>
@@ -1601,7 +1679,7 @@
         <v>1001</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1617,15 +1695,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1640,7 +1721,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -1654,7 +1735,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1663,7 +1744,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1676,13 +1757,15 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" s="3">
         <v>200</v>
@@ -1691,13 +1774,15 @@
         <v>500</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1708,15 +1793,15 @@
         <v>1001</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
@@ -1727,26 +1812,26 @@
         <v>102102</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
         <v>1001</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1762,16 +1847,19 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="20.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1783,13 +1871,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1803,19 +1891,19 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="F2" s="3">
         <v>200</v>
@@ -1829,17 +1917,17 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3">
         <v>200</v>
@@ -1848,21 +1936,21 @@
         <v>1001</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3">
@@ -1872,20 +1960,22 @@
         <v>1001</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3">
         <v>200</v>
@@ -1894,7 +1984,7 @@
         <v>1001</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1913,15 +2003,20 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -1933,16 +2028,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1956,22 +2051,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -1985,20 +2080,20 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G3" s="3">
         <v>200</v>
@@ -2007,24 +2102,24 @@
         <v>1001</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3">
@@ -2034,21 +2129,23 @@
         <v>1001</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3">
         <v>200</v>
@@ -2057,23 +2154,25 @@
         <v>1001</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3">
         <v>123456798</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3">
         <v>200</v>
@@ -2082,7 +2181,7 @@
         <v>102101</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2097,16 +2196,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC7F451-EA0B-481B-AAEE-BD37870611EA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="38.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -2121,10 +2224,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2138,7 +2241,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -2147,10 +2250,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3">
         <v>200</v>
@@ -2164,15 +2267,15 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>200</v>
@@ -2181,21 +2284,21 @@
         <v>1001</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3">
@@ -2205,24 +2308,24 @@
         <v>1001</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3">
         <v>200</v>
@@ -2231,15 +2334,15 @@
         <v>1001</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
@@ -2255,7 +2358,7 @@
         <v>102102</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2274,15 +2377,20 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="20.6640625" style="2" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -2294,16 +2402,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -2317,22 +2425,22 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -2346,20 +2454,20 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3">
         <v>200</v>
@@ -2368,24 +2476,24 @@
         <v>1001</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="3">
@@ -2395,21 +2503,23 @@
         <v>1001</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G5" s="3">
         <v>200</v>
@@ -2418,25 +2528,25 @@
         <v>1001</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3">
         <v>123456798</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3">
         <v>200</v>
@@ -2445,7 +2555,7 @@
         <v>102101</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2461,15 +2571,19 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="20.6640625" style="2" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -2484,10 +2598,10 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -2501,7 +2615,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -2510,10 +2624,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F2" s="3">
         <v>200</v>
@@ -2526,14 +2640,16 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3">
         <v>200</v>
@@ -2542,21 +2658,21 @@
         <v>1001</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3">
@@ -2566,24 +2682,24 @@
         <v>1001</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3">
         <v>200</v>
@@ -2592,15 +2708,15 @@
         <v>1001</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
@@ -2616,7 +2732,7 @@
         <v>102101</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2635,15 +2751,17 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
@@ -2655,7 +2773,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -2669,13 +2787,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -2688,9 +2806,11 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3">
@@ -2700,18 +2820,18 @@
         <v>1001</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -2720,16 +2840,18 @@
         <v>1001</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5" s="3">
         <v>200</v>
@@ -2738,7 +2860,7 @@
         <v>1001</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify iems-subscription-management-test-data.xlsx for the response code of 'iEMS-sub-mgmt-Tes-10' and 'iEMS-sub-mgmt-Test-4'
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-api-service-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F594F69-6D11-48BD-B008-7F4829E6D561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464E0E79-1735-494B-8133-617110CC7033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDevicesByType" sheetId="5" r:id="rId1"/>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76532F20-62D7-47A4-8752-2E5ADEA862B4}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -1292,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08798671-DED1-4851-A8DF-0C914FB8CC5D}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1539,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
@@ -2751,7 +2751,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>

</xml_diff>